<commit_message>
adds models of member, vacancy, jobApplication
</commit_message>
<xml_diff>
--- a/TeamData/Overflow(Lirten)BackLog.xlsx
+++ b/TeamData/Overflow(Lirten)BackLog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="142">
   <si>
     <t xml:space="preserve">Team name</t>
   </si>
@@ -407,19 +407,19 @@
     <t xml:space="preserve">acceptedMember</t>
   </si>
   <si>
+    <t xml:space="preserve">Job Applications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">partner[Entity]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vacancy[Entity]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">member[Entity]</t>
+  </si>
+  <si>
     <t xml:space="preserve">datePosted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Job Applications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">partner[Entity]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vacancy[Entity]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">member[Entity]</t>
   </si>
   <si>
     <t xml:space="preserve">text</t>
@@ -856,10 +856,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -868,15 +864,15 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="B24" activeCellId="1" sqref="7:7 B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="120.724696356275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="121.902834008097"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="2" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="77.3400809716599"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="77.9838056680162"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1456,7 +1452,6 @@
 Scrum email:</oddHeader>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1467,18 +1462,18 @@
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="1" sqref="7:7 D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="2" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.6315789473684"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.165991902834"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1801,28 +1796,28 @@
   </sheetPr>
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="7:7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="14.3522267206478"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.7773279352227"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.2834008097166"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.6356275303644"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.0647773279352"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="31.9230769230769"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="35.9919028340081"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="35.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="14.4615384615385"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.3846153846154"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="36.3117408906883"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="36.3117408906883"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1838,25 +1833,25 @@
       <c r="A3" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="25" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1864,34 +1859,34 @@
       <c r="A4" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="J4" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="K4" s="25" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1899,25 +1894,25 @@
       <c r="A5" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="25" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1937,128 +1932,147 @@
       <c r="E6" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="H6" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" s="25" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="H7" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="J7" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="K7" s="0" t="s">
+      <c r="K7" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="L7" s="0" t="s">
-        <v>127</v>
-      </c>
+      <c r="L7" s="25"/>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="C8" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="D8" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="E8" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="E8" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="25" t="s">
         <v>132</v>
       </c>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="C9" s="0" t="s">
+      <c r="B9" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="E9" s="0" t="s">
-        <v>127</v>
-      </c>
+      <c r="E9" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>127</v>
-      </c>
       <c r="G10" s="26"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="E11" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="F11" s="0" t="s">
+      <c r="E11" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="F11" s="25" t="s">
         <v>141</v>
       </c>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:L75">

</xml_diff>